<commit_message>
updating master taxa trait and habitat list
</commit_message>
<xml_diff>
--- a/_raw_data/xlsx/hab_list.xlsx
+++ b/_raw_data/xlsx/hab_list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="2180" windowWidth="27280" windowHeight="15000" activeTab="1"/>
+    <workbookView xWindow="920" yWindow="540" windowWidth="27280" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="habitat_list" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Deep water</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Deep hard bottom</t>
   </si>
   <si>
-    <t>Dee seamount</t>
-  </si>
-  <si>
-    <t>Deep soft benthic</t>
-  </si>
-  <si>
     <t>Soft slope</t>
   </si>
   <si>
@@ -97,19 +91,6 @@
     <t>* this includes planktic habitat</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>habitat types</t>
-    </r>
-  </si>
-  <si>
     <t>zone</t>
   </si>
   <si>
@@ -132,6 +113,33 @@
   </si>
   <si>
     <t>Hadopelagic</t>
+  </si>
+  <si>
+    <t>Deep seamount</t>
+  </si>
+  <si>
+    <t>Deep soft bottom</t>
+  </si>
+  <si>
+    <t>Estuary</t>
+  </si>
+  <si>
+    <t>* added by Casey</t>
+  </si>
+  <si>
+    <t>Pelagic</t>
+  </si>
+  <si>
+    <t>Subtidal hard bottom</t>
+  </si>
+  <si>
+    <t>hab_type</t>
+  </si>
+  <si>
+    <t>coastal</t>
+  </si>
+  <si>
+    <t>continental shelf</t>
   </si>
 </sst>
 </file>
@@ -198,10 +206,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -521,7 +530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -541,8 +550,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
+      <c r="A1" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -558,121 +567,161 @@
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" s="1" customFormat="1">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -688,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -696,18 +745,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -718,7 +767,7 @@
     </row>
     <row r="3" spans="1:3" ht="15">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>200</v>
@@ -729,7 +778,7 @@
     </row>
     <row r="4" spans="1:3" ht="15">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>700</v>
@@ -740,7 +789,7 @@
     </row>
     <row r="5" spans="1:3" ht="15">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2">
         <v>2000</v>
@@ -751,7 +800,7 @@
     </row>
     <row r="6" spans="1:3" ht="15">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2">
         <v>6000</v>

</xml_diff>